<commit_message>
all lists done, for now. ready to modify scripts to accomodate more ligands
THEREFORE IN THESIS: CREATED TOOL TO SCREEN BINDING POCKETS OF SPECIFIC PDBS AND INCLUDE RELATED LIGANDS
</commit_message>
<xml_diff>
--- a/pdb_source_data/Current List of PDBs_updating.xlsx
+++ b/pdb_source_data/Current List of PDBs_updating.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="227">
   <si>
     <t xml:space="preserve">PDB_ID</t>
   </si>
@@ -527,6 +527,9 @@
     <t xml:space="preserve">1ZJ8</t>
   </si>
   <si>
+    <t xml:space="preserve">NirA protein from tuberculosis</t>
+  </si>
+  <si>
     <t xml:space="preserve">2AOP</t>
   </si>
   <si>
@@ -554,21 +557,167 @@
     <t xml:space="preserve">3mmc</t>
   </si>
   <si>
+    <t xml:space="preserve">3B0G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3VKP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posibly very similar to 3vly/z</t>
+  </si>
+  <si>
     <t xml:space="preserve">Therefore only Nitrite Reductase and Sulfite Reductase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOPE. DON’T USE THE BELOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">---&gt; SAH and SRM very different</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siroheme – SAH structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6P5X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1KYQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4CZC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siroheme decarboxylase NirDL, iron porphyrin thing complexed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFE?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4UN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1V9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2YBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEC LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6VDQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3ORV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6P73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BH5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1BBH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5LFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4CDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2RF7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5KPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5T8W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KINDA SIMILAR TO OTHER CYTOCHROMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1S56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3X15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3WFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4B2N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3E7S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3EAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6W6N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6XNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6R6N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1SP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6OT8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6WZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1JNI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3SJ0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1W2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2OZY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1PBY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2BLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2C1D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -590,9 +739,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +753,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFAFD095"/>
         <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -653,39 +809,51 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -697,12 +865,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Pivot Table Corner" xfId="20"/>
-    <cellStyle name="Pivot Table Value" xfId="21"/>
+    <cellStyle name="Pivot Table Category" xfId="20"/>
+    <cellStyle name="Pivot Table Corner" xfId="21"/>
     <cellStyle name="Pivot Table Field" xfId="22"/>
-    <cellStyle name="Pivot Table Category" xfId="23"/>
+    <cellStyle name="Pivot Table Result" xfId="23"/>
     <cellStyle name="Pivot Table Title" xfId="24"/>
-    <cellStyle name="Pivot Table Result" xfId="25"/>
+    <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -775,13 +943,13 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A112:A120 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,13 +1246,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A120" activeCellId="0" sqref="A112:A120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C156" activeCellId="0" sqref="C156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.19"/>
@@ -1106,19 +1274,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1134,20 +1302,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="3"/>
+      <c r="D7" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -1181,26 +1349,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="D13" s="5" t="s">
+      <c r="B13" s="3"/>
+      <c r="D13" s="0" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -1218,11 +1386,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -1232,7 +1400,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -1240,12 +1408,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="D23" s="5" t="s">
+      <c r="B23" s="3"/>
+      <c r="D23" s="0" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1257,18 +1425,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="D25" s="5" t="s">
+      <c r="B25" s="3"/>
+      <c r="D25" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -1278,18 +1446,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="D29" s="5" t="s">
+      <c r="B29" s="3"/>
+      <c r="D29" s="0" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1301,17 +1469,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -1324,21 +1492,21 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="D34" s="5" t="s">
+      <c r="B34" s="3"/>
+      <c r="D34" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="D35" s="5" t="s">
+      <c r="B35" s="3"/>
+      <c r="D35" s="0" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1350,18 +1518,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="D38" s="5" t="s">
+      <c r="B38" s="3"/>
+      <c r="D38" s="0" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1373,18 +1541,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="D41" s="5" t="s">
+      <c r="B41" s="3"/>
+      <c r="D41" s="0" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1396,18 +1564,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="4"/>
-    </row>
-    <row r="44" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="D44" s="5" t="s">
+      <c r="B44" s="3"/>
+      <c r="D44" s="0" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1422,17 +1590,17 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="4"/>
+      <c r="B47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -1442,30 +1610,30 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="D49" s="5" t="s">
+      <c r="B49" s="3"/>
+      <c r="D49" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="0" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="5" t="s">
+      <c r="B50" s="3"/>
+      <c r="C50" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="0" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1480,24 +1648,24 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="4"/>
-      <c r="D52" s="5" t="s">
+      <c r="B52" s="3"/>
+      <c r="D52" s="0" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="53" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="D53" s="5" t="s">
+      <c r="B53" s="3"/>
+      <c r="D53" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="0" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1509,17 +1677,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="4"/>
-    </row>
-    <row r="56" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="4"/>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
@@ -1532,13 +1700,13 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4"/>
-    </row>
-    <row r="59" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4"/>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1"/>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1"/>
+      <c r="B59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -1548,17 +1716,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
-      <c r="D61" s="5" t="s">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1"/>
+      <c r="B61" s="3"/>
+      <c r="D61" s="0" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="62" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3"/>
-      <c r="B62" s="4"/>
-      <c r="D62" s="5" t="s">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1"/>
+      <c r="B62" s="3"/>
+      <c r="D62" s="0" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1570,17 +1738,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B64" s="4"/>
-    </row>
-    <row r="65" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="4"/>
+      <c r="B65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
@@ -1590,20 +1758,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="s">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="4"/>
-      <c r="C67" s="5" t="s">
+      <c r="B67" s="3"/>
+      <c r="C67" s="0" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="68" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="s">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="4"/>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -1616,13 +1784,13 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3"/>
-      <c r="B70" s="4"/>
-    </row>
-    <row r="71" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3"/>
-      <c r="B71" s="4"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1"/>
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1"/>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
@@ -1635,21 +1803,21 @@
         <v>124</v>
       </c>
     </row>
-    <row r="73" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="5" t="s">
+      <c r="B73" s="3"/>
+      <c r="C73" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="s">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B74" s="4"/>
-      <c r="C74" s="5" t="s">
+      <c r="B74" s="3"/>
+      <c r="C74" s="0" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1661,17 +1829,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="5" t="s">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="0" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="77" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="5" t="s">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="0" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1683,17 +1851,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" s="5" customFormat="true" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
+    <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B79" s="4"/>
-    </row>
-    <row r="80" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="4"/>
+      <c r="B80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
@@ -1724,18 +1892,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="5" t="s">
+      <c r="B85" s="3"/>
+      <c r="C85" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="86" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3"/>
-      <c r="B86" s="4"/>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1"/>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
@@ -1882,21 +2050,24 @@
       <c r="A115" s="0" t="s">
         <v>167</v>
       </c>
+      <c r="B115" s="0" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>164</v>
@@ -1904,51 +2075,277 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>164</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>